<commit_message>
Admin Copy to other outlet
</commit_message>
<xml_diff>
--- a/Admin/Suppliers/Manual testcases/Admin can copy settings in marketlist per item to other outlets 8355.xlsx
+++ b/Admin/Suppliers/Manual testcases/Admin can copy settings in marketlist per item to other outlets 8355.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zm-buyerautomation\Admin\Suppliers\Manual testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7C701FB-A1A1-4A11-B55E-2EC0FB10A78D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB6E9A1-6FBF-42D7-83FE-E0D88B1D7E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{68934006-BE07-4277-942E-95B313C33578}"/>
   </bookViews>
@@ -659,7 +659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A8057B-0A54-4D32-A724-F1B4774D7FD3}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -675,7 +675,7 @@
     <col min="8" max="8" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -882,12 +882,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1100,15 +1097,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F2603EC-1C91-4D5D-B0AE-B870A7BAE878}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF7BA83F-E4B2-48F2-A8E5-CC53BEA7D93F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="014d4624-f59d-44c3-a333-b6c591c77b53"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7c8c12dd-75f8-42a3-90db-eecf595a7e04"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1133,18 +1142,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF7BA83F-E4B2-48F2-A8E5-CC53BEA7D93F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F2603EC-1C91-4D5D-B0AE-B870A7BAE878}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="014d4624-f59d-44c3-a333-b6c591c77b53"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7c8c12dd-75f8-42a3-90db-eecf595a7e04"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
manual testcases for Sprint109
</commit_message>
<xml_diff>
--- a/Admin/Suppliers/Manual testcases/Admin can copy settings in marketlist per item to other outlets 8355.xlsx
+++ b/Admin/Suppliers/Manual testcases/Admin can copy settings in marketlist per item to other outlets 8355.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zm-buyerautomation\Admin\Suppliers\Manual testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB6E9A1-6FBF-42D7-83FE-E0D88B1D7E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3508A966-675B-4BBB-983B-4749657C51F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{68934006-BE07-4277-942E-95B313C33578}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
   <si>
     <t>SL. No</t>
   </si>
@@ -659,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A8057B-0A54-4D32-A724-F1B4774D7FD3}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,6 +835,9 @@
       <c r="F7" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="G7" s="7" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
@@ -854,6 +857,9 @@
       </c>
       <c r="F8" s="5" t="s">
         <v>32</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -882,9 +888,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1097,27 +1106,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF7BA83F-E4B2-48F2-A8E5-CC53BEA7D93F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F2603EC-1C91-4D5D-B0AE-B870A7BAE878}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="014d4624-f59d-44c3-a333-b6c591c77b53"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7c8c12dd-75f8-42a3-90db-eecf595a7e04"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1142,9 +1139,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F2603EC-1C91-4D5D-B0AE-B870A7BAE878}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF7BA83F-E4B2-48F2-A8E5-CC53BEA7D93F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="014d4624-f59d-44c3-a333-b6c591c77b53"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7c8c12dd-75f8-42a3-90db-eecf595a7e04"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>